<commit_message>
update Lý thuyết Chương 01 PHP: Mảng Array
</commit_message>
<xml_diff>
--- a/PHP-Course/BackEnd-PHP/02-ASNT.xlsx
+++ b/PHP-Course/BackEnd-PHP/02-ASNT.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ASNT" sheetId="13" r:id="rId1"/>
     <sheet name="Array(Mảng)" sheetId="14" r:id="rId2"/>
     <sheet name="Mảng liên tục" sheetId="15" r:id="rId3"/>
+    <sheet name="Mảng không liên tục" sheetId="16" r:id="rId4"/>
+    <sheet name="Mảng đa chiều" sheetId="17" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="174">
   <si>
     <t>- Làm sao để biết chúng ta đang thao tác với kiểu dữ liệu nào ?</t>
   </si>
@@ -330,9 +332,6 @@
   </si>
   <si>
     <t>Giá trị</t>
-  </si>
-  <si>
-    <t>Mảng liên tục = Mảng số nguyên</t>
   </si>
   <si>
     <t>[Chỉ số]</t>
@@ -580,12 +579,293 @@
   <si>
     <t>echo $value . "&lt;br/&gt;";</t>
   </si>
+  <si>
+    <t>- Mảng không liên tục = Mảng kết hợp</t>
+  </si>
+  <si>
+    <t>- Là Mảng mà các chỉ số của các phần tử có thể là chuỗi hoặc số</t>
+  </si>
+  <si>
+    <t>- Mảng liên tục = Mảng số nguyên</t>
+  </si>
+  <si>
+    <t>- Mảng liên tục là Mảng mà các chỉ số của các phần tử phải thuộc kiểu số nguyên.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [php] =&gt; PHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [zend] =&gt; Zend FrameWork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [joomla] =&gt; Joomla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [0] =&gt; Item 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [1] =&gt; Item 2</t>
+  </si>
+  <si>
+    <t>Zend FrameWork</t>
+  </si>
+  <si>
+    <t>Item 2</t>
+  </si>
+  <si>
+    <t>KQ:</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>In tất cả các phần tử trong Mảng $course</t>
+  </si>
+  <si>
+    <t>?&gt;</t>
+  </si>
+  <si>
+    <t>        foreach ($course as $key =&gt; $value) {</t>
+  </si>
+  <si>
+    <t>                echo $key . " : " . $value . "&lt;br/&gt;";</t>
+  </si>
+  <si>
+    <t>$course           = array();</t>
+  </si>
+  <si>
+    <t>$course["php"]    = "PHP";</t>
+  </si>
+  <si>
+    <t>$course["zend"]   = "Zend FrameWork";</t>
+  </si>
+  <si>
+    <t>$course["joomla"] = "Joomla";</t>
+  </si>
+  <si>
+    <t>$course[]         = "Item 2";</t>
+  </si>
+  <si>
+    <t>$course[]         = "Item 1";</t>
+  </si>
+  <si>
+    <t>echo "&lt;pre&gt;";</t>
+  </si>
+  <si>
+    <t>print_r($course);</t>
+  </si>
+  <si>
+    <t>echo "&lt;/pre&gt;";</t>
+  </si>
+  <si>
+    <t>echo $course['zend'] . "&lt;br/&gt;";</t>
+  </si>
+  <si>
+    <t>$course           = array("php" =&gt; "PHP", "zend" =&gt; "Zend FrameWork"</t>
+  </si>
+  <si>
+    <t>,"joomla" =&gt; "Joomla",0 =&gt; "Item 1",1 =&gt; "Item 2");</t>
+  </si>
+  <si>
+    <t>php : PHP</t>
+  </si>
+  <si>
+    <t>zend : Zend FrameWork</t>
+  </si>
+  <si>
+    <t>joomla : Joomla</t>
+  </si>
+  <si>
+    <t>0 : Item 1</t>
+  </si>
+  <si>
+    <t>1 : Item 2</t>
+  </si>
+  <si>
+    <t>        } </t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>if (!empty ($course)) {</t>
+  </si>
+  <si>
+    <t>$course = array("php" =&gt; "PHP", "zend" =&gt; "Zend FrameWork"</t>
+  </si>
+  <si>
+    <t>- Mảng đa chiều là Mảng Lồng</t>
+  </si>
+  <si>
+    <t>- Là Mảng mà mỗi phần tử trong Mảng chính có thể là 1 Mảng &amp; mỗi phần tử trong Mảng con lại cũng có thể là 1 Mảng</t>
+  </si>
+  <si>
+    <t>$student["SV001"] = array ("name" =&gt; "John", "sex" =&gt; 1, "score" =&gt; array(4,5,6));</t>
+  </si>
+  <si>
+    <t>$student["SV002"] = array ("name" =&gt; "Peter", "sex" =&gt; 1, "score" =&gt; array(5,6,7));</t>
+  </si>
+  <si>
+    <t>$student["SV003"] = array ("name" =&gt; "Marry", "sex" =&gt; 0, "score" =&gt; array(7,8,9));</t>
+  </si>
+  <si>
+    <t>print_r($student);</t>
+  </si>
+  <si>
+    <t>                        ),</t>
+  </si>
+  <si>
+    <t>                );</t>
+  </si>
+  <si>
+    <t>$student = array (</t>
+  </si>
+  <si>
+    <t>        "SV001" =&gt; array("name"         =&gt; "John",</t>
+  </si>
+  <si>
+    <t>                         "sex"          =&gt; 1,</t>
+  </si>
+  <si>
+    <t>                         "score"        =&gt; array(4,5,6)</t>
+  </si>
+  <si>
+    <t>        "SV002" =&gt; array("name"         =&gt; "Peter",</t>
+  </si>
+  <si>
+    <t>                         "score"        =&gt; array(5,6,7)</t>
+  </si>
+  <si>
+    <t>        "SV003" =&gt; array("name"         =&gt; "Marry",</t>
+  </si>
+  <si>
+    <t>                         "sex"          =&gt; 0,</t>
+  </si>
+  <si>
+    <t>                         "score"        =&gt; array(7,8,9)</t>
+  </si>
+  <si>
+    <t>echo $student["SV002"]["name"] . "&lt;br /&gt;";</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Tên của SV002</t>
+  </si>
+  <si>
+    <t>Điểm môn thứ 2 của SV 003</t>
+  </si>
+  <si>
+    <t>echo $student["SV003"]["score"][1] . "&lt;br /&gt;";</t>
+  </si>
+  <si>
+    <t>Thay đổi tên của SV003  thành Anne</t>
+  </si>
+  <si>
+    <t>$student["SV003"]["name"] = "Anne" . "&lt;br /&gt;";</t>
+  </si>
+  <si>
+    <t>Thay đổi điểm của SV003  môn thứ 2 thành 10</t>
+  </si>
+  <si>
+    <t>$student["SV003"]["score"][1] = 10;</t>
+  </si>
+  <si>
+    <t>Truy xuất ra Tên, Giới tính, Tổng số điểm 3 môn của từng SV</t>
+  </si>
+  <si>
+    <t>John - Boy -15</t>
+  </si>
+  <si>
+    <t>Peter - Boy - 18</t>
+  </si>
+  <si>
+    <t>Marry - Girl - 24</t>
+  </si>
+  <si>
+    <t>if (!empty($student)) {</t>
+  </si>
+  <si>
+    <t>        foreach ($student as $key =&gt; $value) {</t>
+  </si>
+  <si>
+    <t>                $name = $value["name"];</t>
+  </si>
+  <si>
+    <t>                $sex = ($value["sex"]==1) ? "Boy" : "Girl";</t>
+  </si>
+  <si>
+    <t>                $score = $value["score"];</t>
+  </si>
+  <si>
+    <t>                $total = 0;</t>
+  </si>
+  <si>
+    <t>                for ($i=0; $i &lt; count($score); $i++) {</t>
+  </si>
+  <si>
+    <t>                        $total += $score[$i];</t>
+  </si>
+  <si>
+    <t>                $total = array_sum($value["score"]);</t>
+  </si>
+  <si>
+    <t>C3:</t>
+  </si>
+  <si>
+    <r>
+      <t>                echo "Name: " . $name . " - Sex: " .$sex . " - Total score: " . </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$total </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>. "&lt;br /&gt;";</t>
+    </r>
+  </si>
+  <si>
+    <t>                $score = array_sum($value["score"]);</t>
+  </si>
+  <si>
+    <r>
+      <t>                echo "Name: " . $name . " - Sex: " .$sex . " - Total score: " . </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$score</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> . "&lt;br /&gt;";</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -649,6 +929,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -757,7 +1043,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -809,12 +1095,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -829,6 +1109,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1325,7 +1633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
@@ -1796,9 +2104,9 @@
       <c r="E36" s="9"/>
       <c r="F36" s="10"/>
       <c r="H36" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="I36" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="I36" s="33" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1811,13 +2119,13 @@
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="F37" s="10"/>
-      <c r="G37" s="27" t="s">
+      <c r="G37" s="25" t="s">
         <v>56</v>
       </c>
       <c r="H37" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="I37" s="26"/>
+      <c r="I37" s="34"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
@@ -1828,16 +2136,16 @@
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="15"/>
-      <c r="G38" s="27" t="s">
+      <c r="G38" s="25" t="s">
         <v>56</v>
       </c>
       <c r="H38" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="I38" s="26"/>
+      <c r="I38" s="34"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G39" s="27"/>
+      <c r="G39" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1852,8 +2160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,123 +2171,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>63</v>
+      <c r="A1" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="28"/>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="26">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="26">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="26">
         <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G8" s="28"/>
+      <c r="G8" s="26"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="G9" s="28"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="28"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" s="28">
+        <v>66</v>
+      </c>
+      <c r="G11" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" s="28">
+        <v>67</v>
+      </c>
+      <c r="G12" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="28">
+        <v>68</v>
+      </c>
+      <c r="G13" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G14" s="28"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -1989,9 +2302,9 @@
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="30"/>
+        <v>79</v>
+      </c>
+      <c r="C23" s="28"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -2001,7 +2314,7 @@
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="9"/>
@@ -2013,7 +2326,7 @@
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="9"/>
@@ -2025,7 +2338,7 @@
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="9"/>
@@ -2039,7 +2352,7 @@
       <c r="B27" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="31"/>
+      <c r="C27" s="29"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
@@ -2048,7 +2361,7 @@
       <c r="I27" s="15"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="29"/>
+      <c r="B28" s="27"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C29" s="4" t="s">
@@ -2069,7 +2382,7 @@
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -2091,7 +2404,7 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -2103,7 +2416,7 @@
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -2115,7 +2428,7 @@
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -2137,7 +2450,7 @@
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
@@ -2149,7 +2462,7 @@
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
@@ -2164,7 +2477,7 @@
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
@@ -2208,7 +2521,7 @@
       <c r="I42" s="15"/>
     </row>
     <row r="43" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E43" s="33" t="s">
+      <c r="E43" s="31" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2232,14 +2545,14 @@
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="10"/>
-      <c r="E46" s="34" t="s">
+      <c r="E46" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="F46" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="F46" s="32" t="s">
+      <c r="G46" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
@@ -2250,14 +2563,14 @@
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="10"/>
-      <c r="E47" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="F47" s="32" t="s">
+      <c r="E47" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G47" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
@@ -2279,4 +2592,1769 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="25"/>
+      <c r="I4" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="7"/>
+      <c r="L5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="L6" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10"/>
+      <c r="L8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+    </row>
+    <row r="17" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="I17" s="9"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+    </row>
+    <row r="18" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="15"/>
+      <c r="G19" s="25"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G20" s="25"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="K24" s="6"/>
+      <c r="L24" s="7"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="K25" s="9"/>
+      <c r="L25" s="10"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="K26" s="9"/>
+      <c r="L26" s="10"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K27" s="9"/>
+      <c r="L27" s="10"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="K28" s="9"/>
+      <c r="L28" s="10"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="K29" s="9"/>
+      <c r="L29" s="10"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="K30" s="9"/>
+      <c r="L30" s="10"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="K31" s="9"/>
+      <c r="L31" s="10"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="10"/>
+    </row>
+    <row r="33" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="K33" s="9"/>
+      <c r="L33" s="10"/>
+    </row>
+    <row r="34" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="K34" s="9"/>
+      <c r="L34" s="10"/>
+    </row>
+    <row r="35" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="10"/>
+      <c r="J35" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="K35" s="9"/>
+      <c r="L35" s="10"/>
+    </row>
+    <row r="36" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="15"/>
+      <c r="J36" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="K36" s="9"/>
+      <c r="L36" s="10"/>
+    </row>
+    <row r="37" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J37" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="K37" s="14"/>
+      <c r="L37" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="P78" sqref="P78"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="7"/>
+      <c r="M5" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="7"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="10"/>
+      <c r="M6" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="10"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="10"/>
+      <c r="M7" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="10"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="10"/>
+      <c r="M8" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="10"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="10"/>
+      <c r="M9" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="10"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="10"/>
+      <c r="M10" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="10"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="10"/>
+      <c r="M11" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="10"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="10"/>
+      <c r="M12" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="10"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="15"/>
+      <c r="M13" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="10"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M14" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="10"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M15" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="10"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M16" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="10"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M17" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="10"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M18" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="15"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G20" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G23" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>153</v>
+      </c>
+      <c r="I25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7"/>
+      <c r="I26" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="7"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="19"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="10"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
+      <c r="I28" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="10"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="10"/>
+      <c r="I29" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="10"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="15"/>
+      <c r="I30" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="15"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="38" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="38" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="38" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="7"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="10"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="10"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="10"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="10"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="19"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="10"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="10"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="10"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="10"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="10"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="10"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="10"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="14"/>
+      <c r="M50" s="15"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="7"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="10"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="10"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="10"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="10"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="19"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="10"/>
+    </row>
+    <row r="59" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B59" s="43"/>
+      <c r="C59" s="43"/>
+      <c r="D59" s="43"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="43"/>
+      <c r="G59" s="43"/>
+      <c r="H59" s="43"/>
+      <c r="I59" s="43"/>
+      <c r="J59" s="43"/>
+      <c r="K59" s="43"/>
+      <c r="L59" s="43"/>
+      <c r="M59" s="44"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="10"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="14"/>
+      <c r="K61" s="14"/>
+      <c r="L61" s="14"/>
+      <c r="M61" s="15"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="7"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="10"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="10"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="9"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="10"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="9"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="10"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="19"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="9"/>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="10"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B70" s="9"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="10"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" s="9"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
+      <c r="M71" s="10"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B72" s="14"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="14"/>
+      <c r="L72" s="14"/>
+      <c r="M72" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D28:D30"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update Exe-02 Part-01 PHP array 04:20 PM 21/06/2020
</commit_message>
<xml_diff>
--- a/PHP-Course/BackEnd-PHP/02-ASNT.xlsx
+++ b/PHP-Course/BackEnd-PHP/02-ASNT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ASNT" sheetId="13" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Mảng không liên tục" sheetId="16" r:id="rId4"/>
     <sheet name="Mảng đa chiều" sheetId="17" r:id="rId5"/>
     <sheet name="Exe 1" sheetId="18" r:id="rId6"/>
+    <sheet name="Exe2" sheetId="19" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="247">
   <si>
     <t>- Làm sao để biết chúng ta đang thao tác với kiểu dữ liệu nào ?</t>
   </si>
@@ -978,12 +979,125 @@
   <si>
     <t>04</t>
   </si>
+  <si>
+    <t>    $data = file("question.txt") or die("Cannot read file");</t>
+  </si>
+  <si>
+    <t>    array_shift($data);</t>
+  </si>
+  <si>
+    <t>Lầy file &amp; đọc file</t>
+  </si>
+  <si>
+    <t>Xóa đi phần tử đầu tiên</t>
+  </si>
+  <si>
+    <t>$arrayQuestions = array();</t>
+  </si>
+  <si>
+    <t>foreach($data as $key =&gt; $value) {</t>
+  </si>
+  <si>
+    <t>    $tmp                 = explode("|", $value);</t>
+  </si>
+  <si>
+    <t>    $id                  = $tmp[0];</t>
+  </si>
+  <si>
+    <t>    $question            = $tmp[1];</t>
+  </si>
+  <si>
+    <t>    $arrayQuestions[$id] = array("question" =&gt; $question);</t>
+  </si>
+  <si>
+    <t>print_r($arrayQuestions);</t>
+  </si>
+  <si>
+    <t>11|Bạn cảm thấy dễ chịu nhất khi nào?</t>
+  </si>
+  <si>
+    <t>12|Bạn thường bước đi:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [0] =&gt; 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [1] =&gt; Bạn cảm thấy dễ chịu nhất khi nào?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [0] =&gt; 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [1] =&gt; Bạn thường bước đi:</t>
+  </si>
+  <si>
+    <t>    foreach($data as $key =&gt; $value) {</t>
+  </si>
+  <si>
+    <t>    $arrayQuestions[$id] = $question;</t>
+  </si>
+  <si>
+    <t>    $arrayQuestions = array();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [11] =&gt; Bạn cảm thấy dễ chịu nhất khi nào?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [12] =&gt; Bạn thường bước đi:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [31] =&gt; Khi nói chuyện với người khác, bạn:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [43] =&gt; Khi nghỉ ngơi, bạn ngồi như thế nào?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [15] =&gt; Khi ngạc nhiên thích thú, bạn phản ứng thế nào?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [26] =&gt; Khi đi dự tiệc, bạn:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [17] =&gt; Bạn đang làm việc và tập trung cao độ thì bị cắt ngang. Bạn:</t>
+  </si>
+  <si>
+    <r>
+      <t>    $arrayQuestions[$id] = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>array("question" =&gt; $question);</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    [11] =&gt; Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            [question] =&gt; Bạn cảm thấy dễ chịu nhất khi nào?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [12] =&gt; Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            [question] =&gt; Bạn thường bước đi:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1054,6 +1168,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1069,7 +1191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1157,11 +1279,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1243,6 +1391,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1255,8 +1405,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1563,7 +1751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -1753,7 +1941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
@@ -2226,7 +2414,7 @@
       <c r="H36" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="I36" s="41" t="s">
+      <c r="I36" s="43" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2245,7 +2433,7 @@
       <c r="H37" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="I37" s="42"/>
+      <c r="I37" s="44"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
@@ -2262,7 +2450,7 @@
       <c r="H38" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="I38" s="42"/>
+      <c r="I38" s="44"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G39" s="25"/>
@@ -2280,7 +2468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -2718,7 +2906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
@@ -3495,7 +3683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S72"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P78" sqref="P78"/>
     </sheetView>
   </sheetViews>
@@ -3864,7 +4052,7 @@
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="43"/>
+      <c r="D28" s="45"/>
       <c r="E28" s="9"/>
       <c r="F28" s="10"/>
       <c r="I28" s="12" t="s">
@@ -3881,7 +4069,7 @@
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="43"/>
+      <c r="D29" s="45"/>
       <c r="E29" s="9"/>
       <c r="F29" s="10"/>
       <c r="I29" s="12" t="s">
@@ -3898,7 +4086,7 @@
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
-      <c r="D30" s="44"/>
+      <c r="D30" s="46"/>
       <c r="E30" s="14"/>
       <c r="F30" s="15"/>
       <c r="I30" s="38" t="s">
@@ -4483,7 +4671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
@@ -4709,7 +4897,7 @@
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
-      <c r="L14" s="46" t="s">
+      <c r="L14" s="42" t="s">
         <v>197</v>
       </c>
     </row>
@@ -5014,7 +5202,7 @@
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
       <c r="K33" s="14"/>
-      <c r="L33" s="45" t="s">
+      <c r="L33" s="41" t="s">
         <v>196</v>
       </c>
       <c r="M33" s="15"/>
@@ -5401,7 +5589,7 @@
       <c r="I57" s="14"/>
       <c r="J57" s="14"/>
       <c r="K57" s="14"/>
-      <c r="L57" s="45" t="s">
+      <c r="L57" s="41" t="s">
         <v>207</v>
       </c>
       <c r="M57" s="15"/>
@@ -5822,7 +6010,7 @@
       <c r="I83" s="14"/>
       <c r="J83" s="14"/>
       <c r="K83" s="14"/>
-      <c r="L83" s="45" t="s">
+      <c r="L83" s="41" t="s">
         <v>212</v>
       </c>
       <c r="M83" s="15"/>
@@ -5830,4 +6018,1066 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="7"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="10"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="10"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="10"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="10"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>224</v>
+      </c>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="L6" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="53"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="62"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="54" t="s">
+        <v>225</v>
+      </c>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="59"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="58" t="s">
+        <v>226</v>
+      </c>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="59"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="58" t="s">
+        <v>227</v>
+      </c>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="59"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="59"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="59"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="59"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="59"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="59"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="59"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="61" t="s">
+        <v>229</v>
+      </c>
+      <c r="M16" s="55"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="55"/>
+      <c r="P16" s="56"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="15"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="7"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="10"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="10"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="10"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="10"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="10"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="10"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="10"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="10"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="J28" s="48"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="10"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="10"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="10"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="10"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="10"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="10"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="10"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="19"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="10"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="15"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J37" s="47"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="7"/>
+      <c r="J38" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="7"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="10"/>
+      <c r="J39" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="10"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="10"/>
+      <c r="J40" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="10"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="19"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="10"/>
+      <c r="J41" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="10"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="10"/>
+      <c r="J42" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="10"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="19"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="10"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="10"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="J44" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+      <c r="O44" s="10"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="64"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="9"/>
+      <c r="N45" s="9"/>
+      <c r="O45" s="10"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="10"/>
+      <c r="J46" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="10"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="10"/>
+      <c r="J47" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="10"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="10"/>
+      <c r="J48" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="10"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="10"/>
+      <c r="J49" s="48"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="9"/>
+      <c r="O49" s="10"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="10"/>
+      <c r="J50" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="10"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="10"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
+      <c r="O51" s="10"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="15"/>
+      <c r="J52" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="K52" s="14"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="14"/>
+      <c r="N52" s="14"/>
+      <c r="O52" s="15"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J53" s="47"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="I44:I45"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>